<commit_message>
Fixed Excel file paths for Render
</commit_message>
<xml_diff>
--- a/data/faculty_data.xlsx
+++ b/data/faculty_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\AU\Chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\university_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21738FA8-E166-42DA-B0A9-E7CDD1EC55AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7D171B-D99E-48D2-A221-CC11B92ED52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0838F2EC-6C95-4570-815A-5042E62AB961}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="215">
   <si>
     <t xml:space="preserve">Aurora University, Uppal, Hyderabad.
 (Deemed-to-be-University)
@@ -50,38 +50,7 @@
     <t>Department</t>
   </si>
   <si>
-    <t>Dr. C.Srilatha</t>
-  </si>
-  <si>
-    <t>05.11.2022</t>
-  </si>
-  <si>
-    <t>Prof.&amp;VC , ECE, SoE</t>
-  </si>
-  <si>
-    <t>Registrar</t>
-  </si>
-  <si>
-    <t>vc@aurora.edu.in</t>
-  </si>
-  <si>
     <t>School of Engineering</t>
-  </si>
-  <si>
-    <t>Mr.K.Chandrasekhar</t>
-  </si>
-  <si>
-    <t>08.07.2023</t>
-  </si>
-  <si>
-    <t>Assoc.Prof &amp; Registrar, ECE,SoE</t>
-  </si>
-  <si>
-    <t>Director,Evaluation</t>
-  </si>
-  <si>
-    <t>registrar@aurora.edu.in
-doe@aurora.edu.in</t>
   </si>
   <si>
     <t>Mr. A.Anendhar</t>
@@ -865,7 +834,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -885,9 +854,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -899,9 +865,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1319,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334D6599-223A-4FE2-B6C3-425E5B225F15}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39:J44"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1333,10 +1296,10 @@
     <col min="4" max="4" width="22.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.36328125" customWidth="1"/>
     <col min="6" max="6" width="13.08984375" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" style="48" customWidth="1"/>
-    <col min="8" max="8" width="29.08984375" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.453125" style="48" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="29.08984375" style="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.453125" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" style="29" customWidth="1"/>
     <col min="257" max="257" width="6.453125" customWidth="1"/>
     <col min="258" max="258" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="11.1796875" customWidth="1"/>
@@ -1970,25 +1933,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1997,1296 +1960,1234 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8">
+        <v>9100000661</v>
+      </c>
+      <c r="F3" s="9">
+        <v>9100000661</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9">
-        <v>9100666666</v>
-      </c>
-      <c r="F3" s="10">
-        <v>9100666666</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9">
-        <v>9100111111</v>
-      </c>
-      <c r="F4" s="10">
-        <v>9100111111</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="D4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="16">
+        <v>9100000186</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="9"/>
       <c r="J4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="9">
-        <v>9100000661</v>
-      </c>
-      <c r="F5" s="10">
-        <v>9100000661</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="15">
+        <v>9618228942</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>20</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
+        <v>6</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8">
+        <v>9440690710</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9100000110</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="17">
-        <v>9248787084</v>
-      </c>
-      <c r="F6" s="18">
-        <v>9100000186</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="17">
-        <v>9618228942</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="22">
+        <v>8008456008</v>
+      </c>
+      <c r="F7" s="23">
+        <v>9100000117</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="I7" s="12"/>
       <c r="J7" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="E8" s="8">
+        <v>9247448766</v>
+      </c>
+      <c r="F8" s="9">
+        <v>9100000112</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="H8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="9">
-        <v>9440690710</v>
-      </c>
-      <c r="F8" s="10">
-        <v>9100000110</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>35</v>
+      <c r="I8" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
-        <v>7</v>
-      </c>
-      <c r="B9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="E9" s="8">
+        <v>9908392233</v>
+      </c>
+      <c r="F9" s="16">
+        <v>9100000135</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="24">
-        <v>8008456008</v>
-      </c>
-      <c r="F9" s="25">
-        <v>9100000117</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="25" t="s">
+        <v>38</v>
+      </c>
       <c r="J9" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
-        <v>8</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>38</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="9">
-        <v>9247448766</v>
-      </c>
-      <c r="F10" s="10">
-        <v>9100000112</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="D10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="8">
+        <v>7893930391</v>
+      </c>
+      <c r="F10" s="16">
+        <v>9100000174</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="J10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>12</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>9</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="C11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8">
+        <v>9398168896</v>
+      </c>
+      <c r="F11" s="9">
+        <v>9100000150</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="9">
-        <v>9908392233</v>
-      </c>
-      <c r="F11" s="18">
-        <v>9100000135</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>47</v>
       </c>
       <c r="I11" s="27" t="s">
         <v>48</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
-        <v>10</v>
-      </c>
-      <c r="B12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="9">
-        <v>7893930391</v>
-      </c>
-      <c r="F12" s="18">
-        <v>9100000174</v>
-      </c>
-      <c r="G12" s="18"/>
+      <c r="D12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="8">
+        <v>8074223372</v>
+      </c>
+      <c r="F12" s="9">
+        <v>9100000145</v>
+      </c>
+      <c r="G12" s="9"/>
       <c r="H12" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="14" t="s">
         <v>52</v>
       </c>
+      <c r="I12" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="J12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="9">
-        <v>9398168896</v>
-      </c>
-      <c r="F13" s="10">
-        <v>9100000150</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="8">
+        <v>9010124950</v>
+      </c>
+      <c r="F13" s="16">
+        <v>9100000154</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="C14" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="E14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="16">
+        <v>9100000119</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="9">
-        <v>8074223372</v>
-      </c>
-      <c r="F14" s="10">
-        <v>9100000145</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11" t="s">
+      <c r="I14" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>63</v>
-      </c>
       <c r="J14" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="D15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="9">
-        <v>9010124950</v>
-      </c>
-      <c r="F15" s="18">
-        <v>9100000154</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19" t="s">
+      <c r="E15" s="8">
+        <v>9425310640</v>
+      </c>
+      <c r="F15" s="9">
+        <v>9100000120</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>66</v>
+      <c r="H15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="C16" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="18">
-        <v>9100000119</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="E16" s="8">
+        <v>9471529232</v>
+      </c>
+      <c r="F16" s="16">
+        <v>9100000168</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="I16" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="J16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="39" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="9">
-        <v>9425310640</v>
-      </c>
-      <c r="F17" s="10">
-        <v>9100000120</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="E17" s="8">
+        <v>9100888888</v>
+      </c>
+      <c r="F17" s="9">
+        <v>9100888888</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12"/>
+      <c r="J17" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
-        <v>19</v>
-      </c>
-      <c r="B18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="E18" s="15">
+        <v>7989679388</v>
+      </c>
+      <c r="F18" s="16">
+        <v>9100000134</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="9">
-        <v>9471529232</v>
-      </c>
-      <c r="F18" s="18">
-        <v>9100000168</v>
-      </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="39" x14ac:dyDescent="0.35">
+      <c r="J18" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="9">
-        <v>9100888888</v>
-      </c>
-      <c r="F19" s="10">
-        <v>9100888888</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="D19" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="E19" s="15">
+        <v>9652605295</v>
+      </c>
+      <c r="F19" s="16">
+        <v>9100000192</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="31" t="s">
+      <c r="I19" s="19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="J19" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
-        <v>21</v>
-      </c>
-      <c r="B20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="17">
-        <v>7989679388</v>
-      </c>
-      <c r="F20" s="18">
-        <v>9100000134</v>
-      </c>
-      <c r="G20" s="18" t="s">
+      <c r="E20" s="8">
+        <v>9705016213</v>
+      </c>
+      <c r="F20" s="9">
+        <v>9100000129</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="I20" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="J20" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A21" s="5">
+        <v>24</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="25" x14ac:dyDescent="0.35">
-      <c r="A21" s="5">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="22">
+        <v>9440850473</v>
+      </c>
+      <c r="F21" s="23">
+        <v>9100000195</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="17">
-        <v>9652605295</v>
-      </c>
-      <c r="F21" s="18">
-        <v>9100000192</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="32" t="s">
+      <c r="I21" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="I21" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>88</v>
+      <c r="J21" s="29" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
-        <v>23</v>
-      </c>
-      <c r="B22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="8">
+        <v>9705429906</v>
+      </c>
+      <c r="F22" s="9">
+        <v>9100000197</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="9">
-        <v>9705016213</v>
-      </c>
-      <c r="F22" s="10">
-        <v>9100000129</v>
-      </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="I22" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" s="31" t="s">
-        <v>88</v>
+      <c r="J22" s="29" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
-        <v>24</v>
-      </c>
-      <c r="B23" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="D23" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="8">
+        <v>9492092896</v>
+      </c>
+      <c r="F23" s="16">
+        <v>9100000128</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="24">
-        <v>9440850473</v>
-      </c>
-      <c r="F23" s="25">
-        <v>9100000195</v>
-      </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11" t="s">
+      <c r="I23" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="J23" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>27</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="J23" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="5">
-        <v>25</v>
-      </c>
-      <c r="B24" s="15" t="s">
+      <c r="C24" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="D24" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="9">
-        <v>9705429906</v>
-      </c>
-      <c r="F24" s="10">
-        <v>9100000197</v>
-      </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11" t="s">
+      <c r="E24" s="8">
+        <v>7675983554</v>
+      </c>
+      <c r="F24" s="16">
+        <v>9100000125</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="H24" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J24" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="I24" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
-        <v>26</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="C25" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="9">
-        <v>9492092896</v>
-      </c>
-      <c r="F25" s="18">
-        <v>9100000128</v>
-      </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="11" t="s">
+      <c r="E25" s="8">
+        <v>9703328219</v>
+      </c>
+      <c r="F25" s="16">
+        <v>9100000124</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="J25" s="31" t="s">
-        <v>88</v>
+      <c r="J25" s="29" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
-        <v>27</v>
-      </c>
-      <c r="B26" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E26" s="9">
-        <v>7675983554</v>
-      </c>
-      <c r="F26" s="18">
-        <v>9100000125</v>
-      </c>
-      <c r="G26" s="18" t="s">
+      <c r="E26" s="8">
+        <v>9908481470</v>
+      </c>
+      <c r="F26" s="9">
+        <v>9100000189</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="I26" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="J26" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <v>30</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="J26" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="5">
-        <v>28</v>
-      </c>
-      <c r="B27" s="15" t="s">
+      <c r="C27" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E27" s="9">
-        <v>9703328219</v>
-      </c>
-      <c r="F27" s="18">
-        <v>9100000124</v>
-      </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="11" t="s">
+      <c r="E27" s="8">
+        <v>7816001097</v>
+      </c>
+      <c r="F27" s="9">
+        <v>9100000190</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="H27" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="J27" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="I27" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
-        <v>29</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="9">
-        <v>9908481470</v>
-      </c>
-      <c r="F28" s="10">
-        <v>9100000189</v>
-      </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11" t="s">
+      <c r="D28" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I28" s="29" t="s">
+      <c r="E28" s="8">
+        <v>8008307152</v>
+      </c>
+      <c r="F28" s="16">
+        <v>9100000191</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="J28" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="I28" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
-        <v>30</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="9">
-        <v>7816001097</v>
-      </c>
-      <c r="F29" s="10">
-        <v>9100000190</v>
-      </c>
-      <c r="G29" s="10" t="s">
+      <c r="D29" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="E29" s="15">
+        <v>9848456868</v>
+      </c>
+      <c r="F29" s="16">
+        <v>9100000187</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="J29" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J29" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
-        <v>31</v>
-      </c>
-      <c r="B30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="8">
+        <v>8008401624</v>
+      </c>
+      <c r="F30" s="9">
+        <v>9100000144</v>
+      </c>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="37"/>
+      <c r="J30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E30" s="9">
-        <v>8008307152</v>
-      </c>
-      <c r="F30" s="18">
-        <v>9100000191</v>
-      </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:10" ht="52" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
-        <v>32</v>
-      </c>
-      <c r="B31" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E31" s="17">
-        <v>9848456868</v>
-      </c>
-      <c r="F31" s="18">
-        <v>9100000187</v>
-      </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="35" t="s">
+      <c r="E31" s="8">
+        <v>9866357022</v>
+      </c>
+      <c r="F31" s="9">
+        <v>9100000136</v>
+      </c>
+      <c r="G31" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="I31" s="36" t="s">
+      <c r="H31" s="36" t="s">
         <v>147</v>
       </c>
+      <c r="I31" s="37" t="s">
+        <v>148</v>
+      </c>
       <c r="J31" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
-        <v>33</v>
-      </c>
-      <c r="B32" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E32" s="9">
-        <v>8008401624</v>
-      </c>
-      <c r="F32" s="10">
-        <v>9100000144</v>
-      </c>
-      <c r="G32" s="37"/>
+      <c r="E32" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="16">
+        <v>9100000146</v>
+      </c>
+      <c r="G32" s="32"/>
       <c r="H32" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="I32" s="39"/>
+        <v>153</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="J32" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="52" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
-        <v>34</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="D33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="E33" s="9">
-        <v>9866357022</v>
-      </c>
-      <c r="F33" s="10">
-        <v>9100000136</v>
-      </c>
-      <c r="G33" s="37" t="s">
+      <c r="C33" s="26" t="s">
         <v>156</v>
       </c>
+      <c r="D33" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E33" s="8">
+        <v>9945588664</v>
+      </c>
+      <c r="F33" s="16">
+        <v>9100000151</v>
+      </c>
+      <c r="G33" s="32"/>
       <c r="H33" s="38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I33" s="39" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <v>35</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="8">
+        <v>9866902660</v>
+      </c>
+      <c r="F34" s="16">
+        <v>9100000156</v>
+      </c>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="F34" s="18">
-        <v>9100000146</v>
-      </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="40" t="s">
+      <c r="I34" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="I34" s="39" t="s">
-        <v>164</v>
-      </c>
       <c r="J34" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
-        <v>36</v>
-      </c>
-      <c r="B35" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="D35" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8">
+        <v>8367228398</v>
+      </c>
+      <c r="F35" s="16">
+        <v>9100000141</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="E35" s="9">
-        <v>9945588664</v>
-      </c>
-      <c r="F35" s="18">
-        <v>9100000151</v>
-      </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="40" t="s">
+      <c r="I35" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="I35" s="41" t="s">
-        <v>169</v>
-      </c>
       <c r="J35" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
-        <v>37</v>
-      </c>
-      <c r="B36" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E36" s="9">
-        <v>9866902660</v>
-      </c>
-      <c r="F36" s="18">
-        <v>9100000156</v>
-      </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="35" t="s">
+      <c r="E36" s="8">
+        <v>9652045007</v>
+      </c>
+      <c r="F36" s="16">
+        <v>9100000196</v>
+      </c>
+      <c r="G36" s="32"/>
+      <c r="H36" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="42" t="s">
+      <c r="I36" s="43" t="s">
         <v>173</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
-        <v>38</v>
-      </c>
-      <c r="B37" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="E37" s="9">
-        <v>8367228398</v>
-      </c>
-      <c r="F37" s="18">
-        <v>9100000141</v>
-      </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="43" t="s">
+      <c r="E37" s="8">
+        <v>9390016850</v>
+      </c>
+      <c r="F37" s="16">
+        <v>9100000188</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="37" t="s">
         <v>178</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>148</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
-        <v>40</v>
-      </c>
-      <c r="B38" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E38" s="8">
+        <v>9848543293</v>
+      </c>
+      <c r="F38" s="9">
+        <v>9100000115</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="I38" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E38" s="9">
-        <v>9652045007</v>
-      </c>
-      <c r="F38" s="18">
-        <v>9100000196</v>
-      </c>
-      <c r="G38" s="34"/>
-      <c r="H38" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="I38" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
-        <v>41</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="D39" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E39" s="9">
-        <v>9390016850</v>
-      </c>
-      <c r="F39" s="18">
-        <v>9100000188</v>
-      </c>
-      <c r="G39" s="34"/>
-      <c r="H39" s="40" t="s">
+      <c r="C39" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="I39" s="39" t="s">
+      <c r="D39" s="7" t="s">
         <v>188</v>
       </c>
+      <c r="E39" s="8">
+        <v>9550147310</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="I39" s="37" t="s">
+        <v>191</v>
+      </c>
       <c r="J39" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="39" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
-        <v>42</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E40" s="9">
-        <v>9848543293</v>
-      </c>
-      <c r="F40" s="10">
-        <v>9100000115</v>
-      </c>
-      <c r="G40" s="37" t="s">
+      <c r="C40" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="H40" s="38" t="s">
+      <c r="D40" s="6" t="s">
         <v>194</v>
       </c>
+      <c r="E40" s="8">
+        <v>9676539764</v>
+      </c>
+      <c r="F40" s="9">
+        <v>9100000140</v>
+      </c>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36" t="s">
+        <v>195</v>
+      </c>
       <c r="I40" s="39" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
-        <v>43</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E41" s="9">
-        <v>9550147310</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="37" t="s">
+      <c r="D41" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="8">
+        <v>8464096959</v>
+      </c>
+      <c r="F41" s="9">
+        <v>9100000178</v>
+      </c>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="H41" s="38" t="s">
+      <c r="I41" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="I41" s="39" t="s">
+      <c r="J41" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="5">
+        <v>46</v>
+      </c>
+      <c r="B42" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="J41" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="39" x14ac:dyDescent="0.35">
-      <c r="A42" s="5">
-        <v>44</v>
-      </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="D42" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="8">
+        <v>8519980032</v>
+      </c>
+      <c r="F42" s="16">
+        <v>9100000137</v>
+      </c>
+      <c r="G42" s="32"/>
+      <c r="H42" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="E42" s="9">
-        <v>9676539764</v>
-      </c>
-      <c r="F42" s="10">
-        <v>9100000140</v>
-      </c>
-      <c r="G42" s="37"/>
-      <c r="H42" s="38" t="s">
+      <c r="I42" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="I42" s="41" t="s">
-        <v>206</v>
-      </c>
       <c r="J42" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="5">
-        <v>45</v>
-      </c>
-      <c r="B43" s="47" t="s">
-        <v>207</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E43" s="9">
-        <v>8464096959</v>
-      </c>
-      <c r="F43" s="10">
-        <v>9100000178</v>
-      </c>
-      <c r="G43" s="37"/>
-      <c r="H43" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="I43" s="41" t="s">
-        <v>210</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="5">
-        <v>46</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="E44" s="9">
-        <v>8519980032</v>
-      </c>
-      <c r="F44" s="18">
-        <v>9100000137</v>
-      </c>
-      <c r="G44" s="34"/>
-      <c r="H44" s="40" t="s">
-        <v>214</v>
-      </c>
-      <c r="I44" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3294,76 +3195,74 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I17" r:id="rId1" xr:uid="{341D64CB-F071-4BEE-B313-8828866228D4}"/>
-    <hyperlink ref="I8" r:id="rId2" xr:uid="{9D113AF6-FAC8-4046-AF6A-133435E934CD}"/>
-    <hyperlink ref="I5" r:id="rId3" xr:uid="{EEA8B41B-D4E1-4D16-8843-6ED70586B433}"/>
-    <hyperlink ref="I10" r:id="rId4" xr:uid="{6A7194E0-91F1-41EB-9B17-45D3DFD52153}"/>
-    <hyperlink ref="H5" r:id="rId5" xr:uid="{A4C2C836-238E-4273-BB1C-4D6A8D5BEA8C}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{FF235418-01B8-4C0B-A6CA-9C046A14E1CC}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{8E105E3C-84FE-4481-9B34-495A3497CCC6}"/>
-    <hyperlink ref="H17" r:id="rId8" xr:uid="{481AFF9E-9465-40E1-8CB4-65D2978DCB20}"/>
-    <hyperlink ref="H13" r:id="rId9" xr:uid="{194F11FE-D569-45D0-8773-BDCA8609F748}"/>
-    <hyperlink ref="I14" r:id="rId10" xr:uid="{CB961AEF-C68F-4D1B-B61E-E49F37DB4924}"/>
-    <hyperlink ref="H14" r:id="rId11" display="krishnakumari@aurora.edu.in" xr:uid="{B035B902-1B54-4BD1-8FD6-A1706B895409}"/>
-    <hyperlink ref="H4" r:id="rId12" display="doe@aurora.edu.in" xr:uid="{BED9A4CC-428B-450D-B4F6-03DA3DD6B5FA}"/>
-    <hyperlink ref="H11" r:id="rId13" xr:uid="{2B0BFCCB-882E-4E13-BAD7-403B68AAC1F4}"/>
-    <hyperlink ref="I12" r:id="rId14" xr:uid="{396DF1F3-92F5-4243-8790-462F5AE567DE}"/>
-    <hyperlink ref="H3" r:id="rId15" xr:uid="{3FC57BB2-4491-4297-B25B-F93D95E92593}"/>
-    <hyperlink ref="H15" r:id="rId16" xr:uid="{FBAF2A9E-EF18-4D3C-BE2E-6581CFB4A369}"/>
-    <hyperlink ref="I6" r:id="rId17" xr:uid="{FE25B177-A386-4F32-84C6-434AF9A599A0}"/>
-    <hyperlink ref="H6" r:id="rId18" display="aruna@aurora.edu.in" xr:uid="{87FD89F0-FBEF-4CB9-A9F6-BB8C61E0FC14}"/>
-    <hyperlink ref="I11" r:id="rId19" xr:uid="{C4862A39-045F-49A3-98B7-075DCA63EFBA}"/>
-    <hyperlink ref="I13" r:id="rId20" xr:uid="{B0488A11-F3D0-44CF-B77A-36A18A71560F}"/>
-    <hyperlink ref="I15" r:id="rId21" xr:uid="{BF1CA6F2-B401-4803-B35F-494748FE2E00}"/>
-    <hyperlink ref="I16" r:id="rId22" xr:uid="{03A87282-44C4-484A-A3D9-B701E2D1DB90}"/>
-    <hyperlink ref="H16" r:id="rId23" xr:uid="{3C061D6A-A333-44AE-8326-0E4E04065EAF}"/>
-    <hyperlink ref="I7" r:id="rId24" xr:uid="{071E5A59-E255-477F-A6D4-F6B385B062C1}"/>
-    <hyperlink ref="I20" r:id="rId25" xr:uid="{BA6DC187-1AE1-4B50-986E-4D79F29F95AF}"/>
-    <hyperlink ref="I25" r:id="rId26" xr:uid="{98503721-C6BB-4F11-989C-CACF762F9BE7}"/>
-    <hyperlink ref="I26" r:id="rId27" xr:uid="{585D33C6-DF77-4A12-9757-68BD88624BD8}"/>
-    <hyperlink ref="I27" r:id="rId28" xr:uid="{1EDF7CCB-47CA-4D51-9E36-8C21EBED769D}"/>
-    <hyperlink ref="H26" r:id="rId29" xr:uid="{724C0115-F65A-4A79-8A83-58FEBA32D468}"/>
-    <hyperlink ref="H27" r:id="rId30" xr:uid="{41899844-CA6F-4BF6-93EB-E5E3EBAA03D1}"/>
-    <hyperlink ref="H25" r:id="rId31" xr:uid="{31ED8249-B68D-41CD-8442-DF590500AB29}"/>
-    <hyperlink ref="H20" r:id="rId32" display="gita@aurora.edu.in" xr:uid="{7C5038AE-95E7-40A0-90FC-D3BAF5990FD0}"/>
-    <hyperlink ref="H22" r:id="rId33" xr:uid="{89147907-6B8F-4836-9F42-490363B0A85A}"/>
-    <hyperlink ref="I22" r:id="rId34" xr:uid="{7517AD6E-6DA0-4572-B733-57D7298C67B7}"/>
-    <hyperlink ref="I29" r:id="rId35" xr:uid="{45798E4F-F756-4F53-99BD-69702D0D72B7}"/>
-    <hyperlink ref="H29" r:id="rId36" xr:uid="{C4FA00E4-1AF4-47B0-80F8-706FC46E53A7}"/>
-    <hyperlink ref="H30" r:id="rId37" xr:uid="{BD8C90F9-11FD-4F40-B3FD-09EF42EFE063}"/>
-    <hyperlink ref="H28" r:id="rId38" xr:uid="{2373A41C-7D01-4B81-8EEE-AE99550BB39B}"/>
-    <hyperlink ref="H21" r:id="rId39" xr:uid="{32287B3E-D78B-4427-BD30-3790B8ADB372}"/>
-    <hyperlink ref="I21" r:id="rId40" xr:uid="{639E0034-A067-4D8C-B697-A2F195CF02C0}"/>
-    <hyperlink ref="I23" r:id="rId41" xr:uid="{AC872C41-044B-4552-B80E-ADFBE794D861}"/>
-    <hyperlink ref="I28" r:id="rId42" xr:uid="{E1F49DC8-6D70-49C1-BCC5-E806CF22702B}"/>
-    <hyperlink ref="I30" r:id="rId43" xr:uid="{95600D6D-FC5D-4BE5-B459-FBD96F47D1A0}"/>
-    <hyperlink ref="H24" r:id="rId44" xr:uid="{608C9BCF-AFE0-45DF-86E6-15ED90B40D5D}"/>
-    <hyperlink ref="H23" r:id="rId45" xr:uid="{8F78C486-E08D-474A-872F-D9BF083BEA4F}"/>
-    <hyperlink ref="I33" r:id="rId46" xr:uid="{C953BB1A-CCA8-4FA8-8673-5C6C166E6A0E}"/>
-    <hyperlink ref="H33" r:id="rId47" xr:uid="{AC087442-9F95-4D1E-BA6F-943B8B6C809B}"/>
-    <hyperlink ref="I34" r:id="rId48" xr:uid="{3F16645E-7FFA-436E-BD43-2CD3EAED94A1}"/>
-    <hyperlink ref="H34" r:id="rId49" xr:uid="{CDBA9E3B-CC01-4450-A020-70905C3E0887}"/>
-    <hyperlink ref="H35" r:id="rId50" xr:uid="{34F01E80-74F3-4221-B090-6ABD78E0FD8A}"/>
-    <hyperlink ref="I36" r:id="rId51" xr:uid="{DE49D94C-D5B2-4D66-A162-E2C91FE5BB52}"/>
-    <hyperlink ref="I31" r:id="rId52" xr:uid="{77604FA0-3CD3-4544-9567-9BB51DFD224E}"/>
-    <hyperlink ref="H36" r:id="rId53" xr:uid="{4EA7372A-16E5-4B28-B5A5-E126E9194BA7}"/>
-    <hyperlink ref="H31" r:id="rId54" display="sanjaykumar@aurora.edu.in" xr:uid="{8F8310BC-B9EE-4139-8768-B3730F047519}"/>
-    <hyperlink ref="H37" r:id="rId55" display="mailto:shameembegum@aurora.edu.in" xr:uid="{D8162DD1-7A3E-4F27-8106-36A7F28CAE0B}"/>
-    <hyperlink ref="I38" r:id="rId56" xr:uid="{556E757E-252F-4AD4-A831-B78EB0B8BB22}"/>
-    <hyperlink ref="H38" r:id="rId57" xr:uid="{84BAC7E6-ACBB-4977-BBF2-A6A3E856F17E}"/>
-    <hyperlink ref="I35" r:id="rId58" xr:uid="{606CD4E8-29FC-47D8-B856-D2668F311E60}"/>
-    <hyperlink ref="I40" r:id="rId59" xr:uid="{28593938-493D-4512-8700-30219DC4DE3C}"/>
-    <hyperlink ref="I41" r:id="rId60" xr:uid="{F05A5F07-86D3-4D50-91A6-D33028A332E3}"/>
-    <hyperlink ref="H40" r:id="rId61" xr:uid="{F82E688C-0D07-41CC-A8B3-2EA397A04C31}"/>
-    <hyperlink ref="H41" r:id="rId62" xr:uid="{596BCDC5-230E-443F-88E8-CD440AB401EB}"/>
-    <hyperlink ref="H42" r:id="rId63" xr:uid="{D137881E-C38B-4BED-83D6-797FD040BA95}"/>
-    <hyperlink ref="I44" r:id="rId64" xr:uid="{DD0D0055-018E-430D-BE4B-444C56D52409}"/>
-    <hyperlink ref="I42" r:id="rId65" xr:uid="{573FE841-D3E9-45B6-A03B-8776217D1C7B}"/>
-    <hyperlink ref="I43" r:id="rId66" xr:uid="{97C5CADF-6DC3-4674-A4C2-E711B0FD53D4}"/>
-    <hyperlink ref="H9" r:id="rId67" xr:uid="{4E812B19-E3B3-4AE5-9964-447E2B61A574}"/>
-    <hyperlink ref="H19" r:id="rId68" display="rakeshsinghthakur@aurora.edu.in" xr:uid="{182BCB71-4174-4002-A153-5CF8D2AA35B2}"/>
+    <hyperlink ref="I15" r:id="rId1" xr:uid="{341D64CB-F071-4BEE-B313-8828866228D4}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{9D113AF6-FAC8-4046-AF6A-133435E934CD}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{EEA8B41B-D4E1-4D16-8843-6ED70586B433}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{6A7194E0-91F1-41EB-9B17-45D3DFD52153}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{A4C2C836-238E-4273-BB1C-4D6A8D5BEA8C}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{FF235418-01B8-4C0B-A6CA-9C046A14E1CC}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{8E105E3C-84FE-4481-9B34-495A3497CCC6}"/>
+    <hyperlink ref="H15" r:id="rId8" xr:uid="{481AFF9E-9465-40E1-8CB4-65D2978DCB20}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{194F11FE-D569-45D0-8773-BDCA8609F748}"/>
+    <hyperlink ref="I12" r:id="rId10" xr:uid="{CB961AEF-C68F-4D1B-B61E-E49F37DB4924}"/>
+    <hyperlink ref="H12" r:id="rId11" display="krishnakumari@aurora.edu.in" xr:uid="{B035B902-1B54-4BD1-8FD6-A1706B895409}"/>
+    <hyperlink ref="H9" r:id="rId12" xr:uid="{2B0BFCCB-882E-4E13-BAD7-403B68AAC1F4}"/>
+    <hyperlink ref="I10" r:id="rId13" xr:uid="{396DF1F3-92F5-4243-8790-462F5AE567DE}"/>
+    <hyperlink ref="H13" r:id="rId14" xr:uid="{FBAF2A9E-EF18-4D3C-BE2E-6581CFB4A369}"/>
+    <hyperlink ref="I4" r:id="rId15" xr:uid="{FE25B177-A386-4F32-84C6-434AF9A599A0}"/>
+    <hyperlink ref="H4" r:id="rId16" display="aruna@aurora.edu.in" xr:uid="{87FD89F0-FBEF-4CB9-A9F6-BB8C61E0FC14}"/>
+    <hyperlink ref="I9" r:id="rId17" xr:uid="{C4862A39-045F-49A3-98B7-075DCA63EFBA}"/>
+    <hyperlink ref="I11" r:id="rId18" xr:uid="{B0488A11-F3D0-44CF-B77A-36A18A71560F}"/>
+    <hyperlink ref="I13" r:id="rId19" xr:uid="{BF1CA6F2-B401-4803-B35F-494748FE2E00}"/>
+    <hyperlink ref="I14" r:id="rId20" xr:uid="{03A87282-44C4-484A-A3D9-B701E2D1DB90}"/>
+    <hyperlink ref="H14" r:id="rId21" xr:uid="{3C061D6A-A333-44AE-8326-0E4E04065EAF}"/>
+    <hyperlink ref="I5" r:id="rId22" xr:uid="{071E5A59-E255-477F-A6D4-F6B385B062C1}"/>
+    <hyperlink ref="I18" r:id="rId23" xr:uid="{BA6DC187-1AE1-4B50-986E-4D79F29F95AF}"/>
+    <hyperlink ref="I23" r:id="rId24" xr:uid="{98503721-C6BB-4F11-989C-CACF762F9BE7}"/>
+    <hyperlink ref="I24" r:id="rId25" xr:uid="{585D33C6-DF77-4A12-9757-68BD88624BD8}"/>
+    <hyperlink ref="I25" r:id="rId26" xr:uid="{1EDF7CCB-47CA-4D51-9E36-8C21EBED769D}"/>
+    <hyperlink ref="H24" r:id="rId27" xr:uid="{724C0115-F65A-4A79-8A83-58FEBA32D468}"/>
+    <hyperlink ref="H25" r:id="rId28" xr:uid="{41899844-CA6F-4BF6-93EB-E5E3EBAA03D1}"/>
+    <hyperlink ref="H23" r:id="rId29" xr:uid="{31ED8249-B68D-41CD-8442-DF590500AB29}"/>
+    <hyperlink ref="H18" r:id="rId30" display="gita@aurora.edu.in" xr:uid="{7C5038AE-95E7-40A0-90FC-D3BAF5990FD0}"/>
+    <hyperlink ref="H20" r:id="rId31" xr:uid="{89147907-6B8F-4836-9F42-490363B0A85A}"/>
+    <hyperlink ref="I20" r:id="rId32" xr:uid="{7517AD6E-6DA0-4572-B733-57D7298C67B7}"/>
+    <hyperlink ref="I27" r:id="rId33" xr:uid="{45798E4F-F756-4F53-99BD-69702D0D72B7}"/>
+    <hyperlink ref="H27" r:id="rId34" xr:uid="{C4FA00E4-1AF4-47B0-80F8-706FC46E53A7}"/>
+    <hyperlink ref="H28" r:id="rId35" xr:uid="{BD8C90F9-11FD-4F40-B3FD-09EF42EFE063}"/>
+    <hyperlink ref="H26" r:id="rId36" xr:uid="{2373A41C-7D01-4B81-8EEE-AE99550BB39B}"/>
+    <hyperlink ref="H19" r:id="rId37" xr:uid="{32287B3E-D78B-4427-BD30-3790B8ADB372}"/>
+    <hyperlink ref="I19" r:id="rId38" xr:uid="{639E0034-A067-4D8C-B697-A2F195CF02C0}"/>
+    <hyperlink ref="I21" r:id="rId39" xr:uid="{AC872C41-044B-4552-B80E-ADFBE794D861}"/>
+    <hyperlink ref="I26" r:id="rId40" xr:uid="{E1F49DC8-6D70-49C1-BCC5-E806CF22702B}"/>
+    <hyperlink ref="I28" r:id="rId41" xr:uid="{95600D6D-FC5D-4BE5-B459-FBD96F47D1A0}"/>
+    <hyperlink ref="H22" r:id="rId42" xr:uid="{608C9BCF-AFE0-45DF-86E6-15ED90B40D5D}"/>
+    <hyperlink ref="H21" r:id="rId43" xr:uid="{8F78C486-E08D-474A-872F-D9BF083BEA4F}"/>
+    <hyperlink ref="I31" r:id="rId44" xr:uid="{C953BB1A-CCA8-4FA8-8673-5C6C166E6A0E}"/>
+    <hyperlink ref="H31" r:id="rId45" xr:uid="{AC087442-9F95-4D1E-BA6F-943B8B6C809B}"/>
+    <hyperlink ref="I32" r:id="rId46" xr:uid="{3F16645E-7FFA-436E-BD43-2CD3EAED94A1}"/>
+    <hyperlink ref="H32" r:id="rId47" xr:uid="{CDBA9E3B-CC01-4450-A020-70905C3E0887}"/>
+    <hyperlink ref="H33" r:id="rId48" xr:uid="{34F01E80-74F3-4221-B090-6ABD78E0FD8A}"/>
+    <hyperlink ref="I34" r:id="rId49" xr:uid="{DE49D94C-D5B2-4D66-A162-E2C91FE5BB52}"/>
+    <hyperlink ref="I29" r:id="rId50" xr:uid="{77604FA0-3CD3-4544-9567-9BB51DFD224E}"/>
+    <hyperlink ref="H34" r:id="rId51" xr:uid="{4EA7372A-16E5-4B28-B5A5-E126E9194BA7}"/>
+    <hyperlink ref="H29" r:id="rId52" display="sanjaykumar@aurora.edu.in" xr:uid="{8F8310BC-B9EE-4139-8768-B3730F047519}"/>
+    <hyperlink ref="H35" r:id="rId53" display="mailto:shameembegum@aurora.edu.in" xr:uid="{D8162DD1-7A3E-4F27-8106-36A7F28CAE0B}"/>
+    <hyperlink ref="I36" r:id="rId54" xr:uid="{556E757E-252F-4AD4-A831-B78EB0B8BB22}"/>
+    <hyperlink ref="H36" r:id="rId55" xr:uid="{84BAC7E6-ACBB-4977-BBF2-A6A3E856F17E}"/>
+    <hyperlink ref="I33" r:id="rId56" xr:uid="{606CD4E8-29FC-47D8-B856-D2668F311E60}"/>
+    <hyperlink ref="I38" r:id="rId57" xr:uid="{28593938-493D-4512-8700-30219DC4DE3C}"/>
+    <hyperlink ref="I39" r:id="rId58" xr:uid="{F05A5F07-86D3-4D50-91A6-D33028A332E3}"/>
+    <hyperlink ref="H38" r:id="rId59" xr:uid="{F82E688C-0D07-41CC-A8B3-2EA397A04C31}"/>
+    <hyperlink ref="H39" r:id="rId60" xr:uid="{596BCDC5-230E-443F-88E8-CD440AB401EB}"/>
+    <hyperlink ref="H40" r:id="rId61" xr:uid="{D137881E-C38B-4BED-83D6-797FD040BA95}"/>
+    <hyperlink ref="I42" r:id="rId62" xr:uid="{DD0D0055-018E-430D-BE4B-444C56D52409}"/>
+    <hyperlink ref="I40" r:id="rId63" xr:uid="{573FE841-D3E9-45B6-A03B-8776217D1C7B}"/>
+    <hyperlink ref="I41" r:id="rId64" xr:uid="{97C5CADF-6DC3-4674-A4C2-E711B0FD53D4}"/>
+    <hyperlink ref="H7" r:id="rId65" xr:uid="{4E812B19-E3B3-4AE5-9964-447E2B61A574}"/>
+    <hyperlink ref="H17" r:id="rId66" display="rakeshsinghthakur@aurora.edu.in" xr:uid="{182BCB71-4174-4002-A153-5CF8D2AA35B2}"/>
   </hyperlinks>
   <pageMargins left="0.56000000000000005" right="0.70866141732283472" top="0.51181102362204722" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId69"/>
+  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId67"/>
 </worksheet>
 </file>
</xml_diff>